<commit_message>
measures for distribution - phase 1
</commit_message>
<xml_diff>
--- a/measures for distribution/phase 1 - translation and stimuli selection/Moran, Hussey & Hughes - pilot/awareness_1.xlsx
+++ b/measures for distribution/phase 1 - translation and stimuli selection/Moran, Hussey & Hughes - pilot/awareness_1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="5420" windowWidth="26820" windowHeight="17040"/>
+    <workbookView xWindow="4335" yWindow="5415" windowWidth="26820" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" r:id="rId1"/>
@@ -24,22 +24,20 @@
     <t>awareness_1_question_text</t>
   </si>
   <si>
-    <t>Think back to the very first part of the experiment. Did you notice anything out of the ordinary in the way the words and pictures were presented during the surveillance tasks?
-Type your response on the keyboard, it will appear below. 
-Press the return/enter key to finish and move on to the next question.
-NB You must enter at least 20 characters.</t>
+    <t>Denk terug aan het eerste deel van het experiment. Viel je iets op aan de manier waarop de woorden en afbeeldingen werden gepresenteerd tijdens de observatietaak? 
+Typ jouw antwoord met het toetsenbord, het zal onderaan verschijnen. 
+Jouw antwoord moet uit minimum 20 karakters bestaan.</t>
   </si>
   <si>
-    <t>Did you notice anything systematic about how particular words and images appeared together during the surveillance tasks?
-Type your response on the keyboard, it will appear below. 
-Press the return/enter key to finish and move on to the next question.
-NB You must enter at least 20 characters.</t>
+    <t>Viel er jou iets systematisch op in hoe sommige woorden en afbeeldingen samen gepresenteerd werden tijdens de observatietaak?
+Typ jouw antwoord met het toetsenbord, het zal onderaan verschijnen. 
+Jouw antwoord moet uit minimum 20 karakters bestaan</t>
   </si>
   <si>
-    <t>Did you notice anything about the words and images that appeared with certain cartoon creatures? 
-Type your response on the keyboard, it will appear below. 
-Press the return/enter key to finish and move on to the next question.
-NB You must enter at least 20 characters.</t>
+    <t>Viel er jou iets op aan de woorden en afbeeldingen die verschenen bij bepaalde cartoon figuren? 
+Typ jouw antwoord met het toetsenbord, het zal onderaan verschijnen
+Druk nu op de backspace of enter toets om af te sluiten en door te gaan naar de volgende vraag. 
+Jouw antwoord moet uit minimum 20 karakters bestaan</t>
   </si>
 </sst>
 </file>
@@ -572,24 +570,24 @@
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Berekening" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Kop 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Kop 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Neutraal" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notitie" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ongeldig" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Totaal" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Uitvoer" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -893,7 +891,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -907,27 +905,27 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.33203125" customWidth="1"/>
+    <col min="1" max="1" width="89.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="127" customHeight="1">
+    <row r="2" spans="1:1" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="126" customHeight="1">
+    <row r="3" spans="1:1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="117" customHeight="1">
+    <row r="4" spans="1:1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>